<commit_message>
Edit view show table all
</commit_message>
<xml_diff>
--- a/ملفات الاكسل لمشروع التخرج/‏‏plan-subject-دبلوم الصيانة الإلكترونية.xlsx
+++ b/ملفات الاكسل لمشروع التخرج/‏‏plan-subject-دبلوم الصيانة الإلكترونية.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bit\Desktop\tamplete\final\timetable-pro\ملفات الاكسل لمشروع التخرج\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F8D9C7-E475-4CCC-93F4-BDA395286457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEAC66F-5A60-48B8-B641-37E6093AC4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="52">
   <si>
     <t>plan_subject_id</t>
   </si>
@@ -54,94 +54,133 @@
     <t>أول</t>
   </si>
   <si>
-    <t>فصل اول</t>
-  </si>
-  <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>CMP03000</t>
-  </si>
-  <si>
     <t>EEE13109</t>
   </si>
   <si>
-    <t>EEE13106</t>
-  </si>
-  <si>
-    <t>EEE13107</t>
-  </si>
-  <si>
-    <t>EEE33100</t>
-  </si>
-  <si>
-    <t>EEE13204</t>
-  </si>
-  <si>
-    <t>MEE01104</t>
-  </si>
-  <si>
-    <t>EEE13108</t>
-  </si>
-  <si>
-    <t>EEE93100</t>
-  </si>
-  <si>
     <t>BUS01144</t>
   </si>
   <si>
-    <t>EEE13208</t>
-  </si>
-  <si>
-    <t>EEE62200</t>
-  </si>
-  <si>
-    <t>EEE93203</t>
-  </si>
-  <si>
-    <t>EEE93204</t>
-  </si>
-  <si>
-    <t>EEE93202</t>
-  </si>
-  <si>
-    <t>EEE02207</t>
-  </si>
-  <si>
-    <t>BUS02245</t>
-  </si>
-  <si>
-    <t>EEE63209</t>
-  </si>
-  <si>
-    <t>EEE93205</t>
-  </si>
-  <si>
-    <t>EEE93206</t>
-  </si>
-  <si>
-    <t>EEE93207</t>
-  </si>
-  <si>
-    <t>EEE02208</t>
-  </si>
-  <si>
     <t>CMP</t>
   </si>
   <si>
-    <t>CMP03001</t>
-  </si>
-  <si>
-    <t>CMP13263</t>
-  </si>
-  <si>
-    <t>CMP03002</t>
-  </si>
-  <si>
-    <t>CMP03120</t>
-  </si>
-  <si>
-    <t>دبلوم الصيانة الإلكترونية</t>
+    <t>ACD03001</t>
+  </si>
+  <si>
+    <t>CMP03000-T</t>
+  </si>
+  <si>
+    <t>CMP03000-P</t>
+  </si>
+  <si>
+    <t>EEE11107</t>
+  </si>
+  <si>
+    <t>EEE11112</t>
+  </si>
+  <si>
+    <t>EEE13109-T</t>
+  </si>
+  <si>
+    <t>EEE13109-P</t>
+  </si>
+  <si>
+    <t>EEE73100</t>
+  </si>
+  <si>
+    <t>ACD13263</t>
+  </si>
+  <si>
+    <t>EEE82109</t>
+  </si>
+  <si>
+    <t>EEE12108</t>
+  </si>
+  <si>
+    <t>EEE11109</t>
+  </si>
+  <si>
+    <t>EEE11108</t>
+  </si>
+  <si>
+    <t>EEE11206</t>
+  </si>
+  <si>
+    <t>EEE11204</t>
+  </si>
+  <si>
+    <t>EEE82102</t>
+  </si>
+  <si>
+    <t>ACD03000</t>
+  </si>
+  <si>
+    <t>EEE81207</t>
+  </si>
+  <si>
+    <t>EEE83201</t>
+  </si>
+  <si>
+    <t>EEE82202</t>
+  </si>
+  <si>
+    <t>EEE82203</t>
+  </si>
+  <si>
+    <t>EEE81204</t>
+  </si>
+  <si>
+    <t>EEE81209</t>
+  </si>
+  <si>
+    <t>ACD03120</t>
+  </si>
+  <si>
+    <t>ACD03003</t>
+  </si>
+  <si>
+    <t>ACD03002</t>
+  </si>
+  <si>
+    <t>EEE02203</t>
+  </si>
+  <si>
+    <t>EEE63202</t>
+  </si>
+  <si>
+    <t>EEE02206</t>
+  </si>
+  <si>
+    <t>EEE82208</t>
+  </si>
+  <si>
+    <t>EEE62210</t>
+  </si>
+  <si>
+    <t>EEE61211</t>
+  </si>
+  <si>
+    <t>EEE11212</t>
+  </si>
+  <si>
+    <t>EEE81211</t>
+  </si>
+  <si>
+    <t>BUS02245-T</t>
+  </si>
+  <si>
+    <t>BUS02245-P</t>
+  </si>
+  <si>
+    <t>EEE13106-T</t>
+  </si>
+  <si>
+    <t>EEE13106-P</t>
+  </si>
+  <si>
+    <t>EEE13107-T</t>
+  </si>
+  <si>
+    <t>EEE13107-P</t>
   </si>
 </sst>
 </file>
@@ -466,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -503,7 +542,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -512,7 +551,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -520,7 +559,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -529,7 +568,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -537,7 +576,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -546,7 +585,7 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -554,7 +593,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -563,7 +602,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -571,16 +610,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -588,33 +627,33 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>10</v>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -622,7 +661,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -631,7 +670,7 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -639,7 +678,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -648,7 +687,7 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -656,7 +695,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -665,7 +704,7 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -673,7 +712,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -682,7 +721,7 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -690,7 +729,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -699,7 +738,7 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -707,7 +746,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -716,7 +755,7 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -724,7 +763,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -733,7 +772,24 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -741,16 +797,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -758,16 +814,16 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -775,33 +831,16 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>18</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -809,7 +848,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -818,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -826,7 +865,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -835,7 +874,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -843,7 +882,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -852,7 +891,24 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>395</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -860,16 +916,16 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -877,16 +933,16 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -894,16 +950,16 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -911,16 +967,16 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -928,16 +984,16 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -945,16 +1001,373 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
         <v>38</v>
       </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
-      <c r="E31" t="s">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>43</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>49</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>